<commit_message>
Add Icon & Update doc
</commit_message>
<xml_diff>
--- a/001_GPSCamera_Document/002＿GPSカメラアプリ＿要求.xlsx
+++ b/001_GPSCamera_Document/002＿GPSカメラアプリ＿要求.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="1" r:id="rId1"/>
@@ -1439,7 +1439,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1477,6 +1477,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1633,7 +1639,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1740,6 +1746,8 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="どちらでもない" xfId="2" builtinId="28"/>
@@ -2049,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.15"/>
@@ -2998,8 +3006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:X41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3551,17 +3559,17 @@
       <c r="K21" s="27"/>
       <c r="L21" s="28"/>
       <c r="N21" s="35"/>
-      <c r="O21" s="36" t="s">
+      <c r="O21" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
-      <c r="V21" s="27"/>
-      <c r="W21" s="27"/>
+      <c r="P21" s="56"/>
+      <c r="Q21" s="56"/>
+      <c r="R21" s="56"/>
+      <c r="S21" s="56"/>
+      <c r="T21" s="56"/>
+      <c r="U21" s="56"/>
+      <c r="V21" s="56"/>
+      <c r="W21" s="56"/>
       <c r="X21" s="28"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.15">
@@ -3622,17 +3630,17 @@
     </row>
     <row r="24" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B24" s="29"/>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
       <c r="L24" s="28"/>
       <c r="N24" s="37"/>
       <c r="O24" s="36" t="s">
@@ -3650,17 +3658,17 @@
     </row>
     <row r="25" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B25" s="29"/>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
       <c r="L25" s="28"/>
       <c r="N25" s="35"/>
       <c r="O25" s="36" t="s">

</xml_diff>